<commit_message>
SQL INSERT INTO a funcionar
</commit_message>
<xml_diff>
--- a/Utils/Campus_2_A_Park1.xlsx
+++ b/Utils/Campus_2_A_Park1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marisa/Documents/ProjetoIS/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE6CB51-801A-BA47-A107-69843E59294F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="6500" windowWidth="28040" windowHeight="17440" xr2:uid="{E9C09612-09AF-3E4B-99D2-8B8D15F60D70}"/>
+    <workbookView xWindow="10656" yWindow="6504" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Campus_2_A_Park1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -90,12 +84,6 @@
     <t>39.734909,-8.820708</t>
   </si>
   <si>
-    <t>39,734905,-8.820718</t>
-  </si>
-  <si>
-    <t>39,734928,-8.820685</t>
-  </si>
-  <si>
     <t>39.734946,-8.820649</t>
   </si>
   <si>
@@ -133,12 +121,18 @@
   </si>
   <si>
     <t>Location (Geo):</t>
+  </si>
+  <si>
+    <t>39.734928,-8.820685</t>
+  </si>
+  <si>
+    <t>39.734905,-8.820718</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
@@ -243,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -295,7 +289,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -489,35 +483,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0941C8BF-080F-0841-8CAE-654BE7571C9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="173" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -533,15 +527,15 @@
         <v>43396.604166666664</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -549,7 +543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -557,7 +551,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -565,100 +559,100 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>